<commit_message>
add audio and location
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/Audio.xlsx
+++ b/data/Spreadsheet_Data/Audio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B084B848-9FC1-3343-961A-9819925D99F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0764F25-5E6B-C841-8F05-9BB158A6A4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26600" yWindow="12620" windowWidth="28040" windowHeight="17440" xr2:uid="{B43DECCB-7160-C844-BDA3-E6330E4A253D}"/>
+    <workbookView xWindow="25060" yWindow="3440" windowWidth="40800" windowHeight="27260" xr2:uid="{B43DECCB-7160-C844-BDA3-E6330E4A253D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -48,16 +47,771 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Time Stamp</t>
+  </si>
+  <si>
+    <t>Copyright</t>
+  </si>
+  <si>
+    <t>License List</t>
+  </si>
+  <si>
+    <t>A_01</t>
+  </si>
+  <si>
+    <t>A_02</t>
+  </si>
+  <si>
+    <t>A_03</t>
+  </si>
+  <si>
+    <t>A_04</t>
+  </si>
+  <si>
+    <t>A_05</t>
+  </si>
+  <si>
+    <t>A_06</t>
+  </si>
+  <si>
+    <t>A_07</t>
+  </si>
+  <si>
+    <t>A_08</t>
+  </si>
+  <si>
+    <t>A_09</t>
+  </si>
+  <si>
+    <t>A_10</t>
+  </si>
+  <si>
+    <t>A_11</t>
+  </si>
+  <si>
+    <t>A_12</t>
+  </si>
+  <si>
+    <t>A_13</t>
+  </si>
+  <si>
+    <t>PDM 1.0</t>
+  </si>
+  <si>
+    <t>Dramatis Personae
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>Down the Rabbit-Hole
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>The Pool of Tears
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>Advice From a Caterpillar
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>Pig and Pepper
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>The Mad Tea-Party
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>The Queen's Croquet-Ground
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>The Mock Turtle's Story
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>The Lobster Quadrille
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>Who Stole the Tarts?
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>Alice's Evidence
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English</t>
+  </si>
+  <si>
+    <t>A Caucus-Race and Long Tale
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English"</t>
+  </si>
+  <si>
+    <t>The Rabbit Sends in a Little Bill
+Alice's Adventures in Wonderland (Dramatic Reading)
+Lewis Carroll (1832 - 1898)
+This classic tale by Lewis Carroll has delighted children for generations. Alice falls down a rabbit hole and encounters a wide variety of strange and wonderful creatures in all manner of bizarre situations. Join Alice as she journeys through Wonderland, trying to make sense of what she finds there. This version is read dramatically, with different readers voicing the different characters. (Summary by Lucy Perry)
+Cast
+Narrator: David Goldfarb
+Alice: Miss Avarice
+The White Rabbit: BellonaTimes
+Mouse: cher0520
+Lory: Availle
+Duck: Jessamy Gloor
+Dodo: Tim Ferreira
+Eaglet: Dennis D.
+Old Crab: Joshua Logan
+Young Crab: Sonja
+Magpie: Lucy Perry
+Canary: ElleyKat
+Pat: Terence Taylor
+Bill: Aidan Brack
+Guinea Pig 1: Rat King
+Guinea Pig 2: Kelseigh
+Caterpillar: Algy Pug
+Pigeon: Kelseigh
+Fish-Footman: Terence
+Frog-Footman: Peter Yearsley
+Cook: Ana
+Baby: Elizabeth Klett
+Duchess: Heather Phillips
+Cheshire Cat: Elizabeth Klett
+March Hare: Denny Sayers
+Hatter: Arielle Lipshaw
+Dormouse: Ruth Golding
+Five: Neeru Iyer
+Two: Elli
+Seven: Henry Frigon
+Soldier 1: Dennis D.
+Soldier 2: Philbert
+Soldier 3: Lucy Perry
+Queen of Hearts: Nadine Eckert-Boulet
+King of Hearts: Peter Yearsley
+Gryphon: Algy Pug
+Mock Turtle: Kara Shallenberg
+Knave of Hearts: Levi Throckmorton
+Alice's Sister: Diana Majlinger
+Audio edited by Elizabeth Klett and Arielle Lipshaw
+Genre(s): Children's Fiction, Dramatic Readings, Fantasy Fiction
+Language: English"</t>
+  </si>
+  <si>
+    <t>data/Multimedia_Data/Audio/</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_00_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_01_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_02_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_03_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_04_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_05_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_06_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_07_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_08_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_09_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_10_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_11_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>aliceinwonderland_12_carroll_64kb.mp3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,13 +834,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,29 +1186,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56BEE1F-058C-DF44-80E1-DAB20F6DF233}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Data Model and XML file
</commit_message>
<xml_diff>
--- a/data/Spreadsheet_Data/Audio.xlsx
+++ b/data/Spreadsheet_Data/Audio.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/data/Spreadsheet_Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/data/Spreadsheet_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0764F25-5E6B-C841-8F05-9BB158A6A4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16F1495D-9766-6E4C-A10C-D40ABF1E22CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25060" yWindow="3440" windowWidth="40800" windowHeight="27260" xr2:uid="{B43DECCB-7160-C844-BDA3-E6330E4A253D}"/>
+    <workbookView xWindow="10960" yWindow="1520" windowWidth="51620" windowHeight="27260" xr2:uid="{B43DECCB-7160-C844-BDA3-E6330E4A253D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>ID</t>
   </si>
@@ -777,6 +778,51 @@
   </si>
   <si>
     <t>aliceinwonderland_12_carroll_64kb.mp3</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Dramatis Personae</t>
+  </si>
+  <si>
+    <t>Down the Rabbit-Hole</t>
+  </si>
+  <si>
+    <t>The Pool of Tears</t>
+  </si>
+  <si>
+    <t>A Caucus-Race and Long Tale</t>
+  </si>
+  <si>
+    <t>The Rabbit Sends in a Little Bill</t>
+  </si>
+  <si>
+    <t>Advice From a Caterpillar</t>
+  </si>
+  <si>
+    <t>Pig and Pepper</t>
+  </si>
+  <si>
+    <t>The Mad Tea-Party</t>
+  </si>
+  <si>
+    <t>The Queen's Croquet-Ground</t>
+  </si>
+  <si>
+    <t>The Mock Turtle's Story</t>
+  </si>
+  <si>
+    <t>The Lobster Quadrille</t>
+  </si>
+  <si>
+    <t>Who Stole the Tarts?</t>
+  </si>
+  <si>
+    <t>Alice's Evidence</t>
+  </si>
+  <si>
+    <t>to be filled</t>
   </si>
 </sst>
 </file>
@@ -838,9 +884,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1186,28 +1231,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E56BEE1F-058C-DF44-80E1-DAB20F6DF233}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="37.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="75.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
@@ -1222,16 +1267,22 @@
       <c r="G1" t="s">
         <v>2</v>
       </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
@@ -1239,16 +1290,22 @@
       <c r="G2" t="s">
         <v>34</v>
       </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
@@ -1256,16 +1313,22 @@
       <c r="G3" t="s">
         <v>34</v>
       </c>
+      <c r="H3" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>62</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
@@ -1273,16 +1336,22 @@
       <c r="G4" t="s">
         <v>34</v>
       </c>
+      <c r="H4" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1290,16 +1359,22 @@
       <c r="G5" t="s">
         <v>34</v>
       </c>
+      <c r="H5" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
@@ -1307,16 +1382,22 @@
       <c r="G6" t="s">
         <v>34</v>
       </c>
+      <c r="H6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -1324,16 +1405,22 @@
       <c r="G7" t="s">
         <v>34</v>
       </c>
+      <c r="H7" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>62</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -1341,16 +1428,22 @@
       <c r="G8" t="s">
         <v>34</v>
       </c>
+      <c r="H8" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>62</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -1358,16 +1451,22 @@
       <c r="G9" t="s">
         <v>34</v>
       </c>
+      <c r="H9" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>62</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
@@ -1375,16 +1474,22 @@
       <c r="G10" t="s">
         <v>34</v>
       </c>
+      <c r="H10" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>28</v>
+      </c>
+      <c r="E11" t="s">
+        <v>62</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1392,16 +1497,22 @@
       <c r="G11" t="s">
         <v>34</v>
       </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -1409,16 +1520,22 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>30</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -1426,22 +1543,31 @@
       <c r="G13" t="s">
         <v>34</v>
       </c>
+      <c r="H13" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>62</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" t="s">
         <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>